<commit_message>
fix: apply WFH recommendation to all Fridays regardless of attendance
Changes:
- Remove incorrect logic that skipped Friday attendance analysis
- Apply WFH suggestion (9 hours) to all Fridays with or without punch records
- Exception: National holidays on Friday are not recommended for WFH
- Update test expectations to match new Friday behavior

Documentation updates:
- CLAUDE.md: Update business rules and issue classification
- README.md: Emphasize Friday WFH policy
- AGENTS.md: Add testing guidelines for Friday WFH
- docs/: Sync all documentation (logic.md, overview.md, data-format.md)

Test results:
- All 120 unit tests passing
- Friday WFH edge cases verified
- Sample data analysis updated

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/sample-attendance-data_analysis.xlsx
+++ b/sample-attendance-data_analysis.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,50 +25,16 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00366092"/>
-        <bgColor rgb="00366092"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E6F3FF"/>
-        <bgColor rgb="00E6F3FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E6FFE6"/>
-        <bgColor rgb="00E6FFE6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFF0E6"/>
-        <bgColor rgb="00FFF0E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFE6E6"/>
-        <bgColor rgb="00FFE6E6"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -76,37 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -479,392 +420,384 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="35" customWidth="1" min="6" max="6"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>日期</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>類型</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>時長(分鐘)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>說明</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>時段</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>計算式</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>2025/07/01</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>加班</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" t="n">
         <v>120</v>
       </c>
-      <c r="D2" s="4" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>加班2小時0分鐘 💼</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>19:28~21:33</t>
         </is>
       </c>
-      <c r="F2" s="4" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>預期下班: 19:28, 實際下班: 21:33, 實際加班: 125分鐘, 可申請: 120分鐘</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>2025/07/04</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>WFH假</t>
         </is>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" t="n">
         <v>540</v>
       </c>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>建議申請整天WFH假 🏠💻</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr"/>
-      <c r="F3" s="4" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>2025/07/08</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>忘刷卡</t>
         </is>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>遲到2分鐘，建議使用忘刷卡 🔄✅</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>10:30~10:32</t>
         </is>
       </c>
-      <c r="F4" s="4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>實際上班: 10:32, 最晚上班: 10:30, 遲到: 2分鐘 (使用忘刷卡，本月剩餘: 1次)</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>2025/07/11</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>WFH假</t>
         </is>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" t="n">
         <v>540</v>
       </c>
-      <c r="D5" s="4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>建議申請整天WFH假 🏠💻</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr"/>
-      <c r="F5" s="4" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>2025/07/15</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>請假</t>
         </is>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" t="n">
         <v>480</v>
       </c>
-      <c r="D6" s="4" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>整天沒進公司，建議請假 📝🏠</t>
         </is>
       </c>
-      <c r="E6" s="2" t="inlineStr"/>
-      <c r="F6" s="4" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>2025/07/18</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>WFH假</t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" t="n">
         <v>540</v>
       </c>
-      <c r="D7" s="4" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>建議申請整天WFH假 🏠💻</t>
         </is>
       </c>
-      <c r="E7" s="2" t="inlineStr"/>
-      <c r="F7" s="4" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>2025/07/21</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>加班</t>
         </is>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" t="n">
         <v>60</v>
       </c>
-      <c r="D8" s="4" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>加班1小時0分鐘 💼</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>19:15~21:13</t>
         </is>
       </c>
-      <c r="F8" s="4" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>預期下班: 19:15, 實際下班: 21:13, 實際加班: 118分鐘, 可申請: 60分鐘</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>2025/07/22</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>遲到</t>
         </is>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" t="n">
         <v>221</v>
       </c>
-      <c r="D9" s="4" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>遲到221分鐘 ⏱️ (超過1小時)</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>10:30~15:11</t>
         </is>
       </c>
-      <c r="F9" s="4" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>實際上班: 15:11, 最晚上班: 10:30, 遲到: 281分鐘 - 60分鐘午休 = 221分鐘</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>2025/07/23</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>加班</t>
         </is>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" t="n">
         <v>60</v>
       </c>
-      <c r="D10" s="4" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>加班1小時0分鐘 💼</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>19:24~20:41</t>
         </is>
       </c>
-      <c r="F10" s="4" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>預期下班: 19:24, 實際下班: 20:41, 實際加班: 77分鐘, 可申請: 60分鐘</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>2025/07/25</t>
         </is>
       </c>
-      <c r="B11" s="5" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>WFH假</t>
         </is>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" t="n">
         <v>540</v>
       </c>
-      <c r="D11" s="4" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>建議申請整天WFH假 🏠💻</t>
         </is>
       </c>
-      <c r="E11" s="2" t="inlineStr"/>
-      <c r="F11" s="4" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>2025/07/28</t>
         </is>
       </c>
-      <c r="B12" s="6" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>忘刷卡</t>
         </is>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" t="n">
         <v>0</v>
       </c>
-      <c r="D12" s="4" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>遲到1分鐘，建議使用忘刷卡 🔄✅</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>10:30~10:31</t>
         </is>
       </c>
-      <c r="F12" s="4" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>實際上班: 10:31, 最晚上班: 10:30, 遲到: 1分鐘 (使用忘刷卡，本月剩餘: 0次)</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>2025/07/28</t>
         </is>
       </c>
-      <c r="B13" s="3" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>加班</t>
         </is>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" t="n">
         <v>60</v>
       </c>
-      <c r="D13" s="4" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>加班1小時0分鐘 💼</t>
         </is>
       </c>
-      <c r="E13" s="2" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>19:31~20:49</t>
         </is>
       </c>
-      <c r="F13" s="4" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>預期下班: 19:31, 實際下班: 20:49, 實際加班: 78分鐘, 可申請: 60分鐘</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>2025/07/29</t>
         </is>
       </c>
-      <c r="B14" s="7" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>遲到</t>
         </is>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" t="n">
         <v>138</v>
       </c>
-      <c r="D14" s="4" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>遲到138分鐘 ⏱️ (超過1小時)</t>
         </is>
       </c>
-      <c r="E14" s="2" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>10:30~13:48</t>
         </is>
       </c>
-      <c r="F14" s="4" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>實際上班: 13:48, 最晚上班: 10:30, 遲到: 198分鐘 - 60分鐘午休 = 138分鐘</t>
         </is>

</xml_diff>